<commit_message>
Spool Holder Bom updated with STL links
</commit_message>
<xml_diff>
--- a/bom/BOM_SpoolHolder.xlsx
+++ b/bom/BOM_SpoolHolder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5DE52998-0904-4BEE-9999-B40C2CDF348E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A98B207B-2102-44D5-9294-8C18596D62D3}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5DE52998-0904-4BEE-9999-B40C2CDF348E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F63FA4BC-E1A1-4AE6-B7A6-7382FF14384C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -124,13 +124,22 @@
   <si>
     <t>This Spool holder integrates a magnetic braking system that provides a very subbltle spin resistance.  Just enough to prevent unwanted filament unroll, but not enough to disrupt your precise extrusion consistency ;)  
 Happy Printing</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/SpoolHolder/FrameBracket.stl</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/SpoolHolder/SpoolRollBody.stl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +251,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -360,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -372,9 +389,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -386,9 +400,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -419,9 +430,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -442,13 +450,130 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFFFFF00"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -489,105 +614,6 @@
           <color rgb="FFFFFF00"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFFFFF00"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1004,24 +1030,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8609672A-97E6-44A7-ABD8-E635700679ED}" name="Table1" displayName="Table1" ref="A2:K9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8609672A-97E6-44A7-ABD8-E635700679ED}" name="Table1" displayName="Table1" ref="A2:K9" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="A2:K9" xr:uid="{8609672A-97E6-44A7-ABD8-E635700679ED}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{57E60FC7-E80F-4365-951C-74E96008894D}" name="SubAssy"/>
-    <tableColumn id="2" xr3:uid="{BCAF809F-B913-43F1-B1AB-32A13D6044B4}" name="Category" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{BCAF809F-B913-43F1-B1AB-32A13D6044B4}" name="Category" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Make/Buy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{495674A0-D886-4FC0-8901-5BB97645BE90}" name="Item" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{D8F55544-7A89-4DBC-A712-EDE57A78404C}" name="Thumbnail" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{22B024A7-C222-4616-AE96-D824A8E91893}" name="Part Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{060E5428-CE42-49F1-8DEA-ACDA937B32A4}" name="Part Description" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{6BDABD36-A994-4CCA-A832-EBA260FE5921}" name="Make/Buy" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{62A1A40A-B650-4727-AB30-BC236368F9D6}" name="QTY" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{495674A0-D886-4FC0-8901-5BB97645BE90}" name="Item" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D8F55544-7A89-4DBC-A712-EDE57A78404C}" name="Thumbnail" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{22B024A7-C222-4616-AE96-D824A8E91893}" name="Part Name" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{060E5428-CE42-49F1-8DEA-ACDA937B32A4}" name="Part Description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6BDABD36-A994-4CCA-A832-EBA260FE5921}" name="Make/Buy" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{62A1A40A-B650-4727-AB30-BC236368F9D6}" name="QTY" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{FA109C1A-53D6-4FA9-9ADD-A809711CA672}" name="Comment"/>
-    <tableColumn id="10" xr3:uid="{487EEDD0-D25F-4B5D-B3FC-BD215049CFB0}" name="Vendor"/>
+    <tableColumn id="10" xr3:uid="{487EEDD0-D25F-4B5D-B3FC-BD215049CFB0}" name="Vendor" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{200CD42D-1EE6-4FC9-95B5-3EACAE6FC89F}" name="Vendor URL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1318,285 +1344,297 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="46.453125" customWidth="1"/>
+    <col min="6" max="6" width="48.453125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="39.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" customWidth="1"/>
-    <col min="11" max="11" width="37.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="39.54296875" customWidth="1"/>
+    <col min="10" max="10" width="24.26953125" customWidth="1"/>
+    <col min="11" max="11" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="14" t="str">
+      <c r="E1" s="12" t="str">
         <f>HYPERLINK("https://a360.co/3RA8JKJ","LINK TO CAD")</f>
         <v>LINK TO CAD</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="14" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="14">
         <v>2</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="11" t="str">
+      <c r="B4" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="11" t="str">
+      <c r="B5" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>3</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>9</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>4</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>2</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="11" t="str">
+      <c r="B7" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>3</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="11" t="str">
+      <c r="B8" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Make</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>6</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>1</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="11" t="str">
+      <c r="B9" s="9" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Make</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>1</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K9" r:id="rId1" xr:uid="{3F7FFA69-C08E-4A5C-952F-6BA8496AA261}"/>
+    <hyperlink ref="K8" r:id="rId2" xr:uid="{984FFBAE-BE2A-40F0-9904-22233FB5C0C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
   <webPublishItems count="1">
     <webPublishItem id="12887" divId="BOM_SpoolHolder_12887" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_SpoolHolder.htm"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>